<commit_message>
minor update of conversion map.
</commit_message>
<xml_diff>
--- a/docs/Developer documentation/ConversionMap-Spreadsheets-MicrosoftOffice_Excel-OpenOffice.org_Calc(-functions).xlsx
+++ b/docs/Developer documentation/ConversionMap-Spreadsheets-MicrosoftOffice_Excel-OpenOffice.org_Calc(-functions).xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="795">
   <si>
     <t>p.: 2533 (sect.: 3.17.7.1)</t>
   </si>
@@ -2476,10 +2476,6 @@
 note: ISLEAPYEAR(B1) = (DATEDIF(DATE(YEAR(B1);2;1);DATE(YEAR(B1);3;1);"D")=29)</t>
   </si>
   <si>
-    <t xml:space="preserve">Name of function changed.
-note: unit conversion function in Excel is named CONVERT, while in OOo it is named CONVERT_ADD ***. It is important not to confuse it with Ooo CONVERT, which converts European currencies. </t>
-  </si>
-  <si>
     <t>CONVERT_ADD</t>
   </si>
   <si>
@@ -2518,6 +2514,14 @@
   </si>
   <si>
     <t>Number of Excel only functions, that can't be mapped**** to Calc functions:</t>
+  </si>
+  <si>
+    <t>Can be converted to OpenOffice.org Calc according to following formula:
+RANDBETWEEN(A1,A2) = A1+INT(RAND(A2))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of function changed.
+note: unit conversion function in Excel is named CONVERT, while in OOo it is named CONVERT_ADD. It is important not to confuse it with Ooo CONVERT, which converts European currencies. </t>
   </si>
 </sst>
 </file>
@@ -3325,7 +3329,104 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF297A00"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF297A00"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF297A00"/>
@@ -3668,8 +3769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:M431"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A395" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="A415" sqref="A415:XFD415"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A399" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="F427" sqref="F427"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5011,12 +5112,12 @@
       <c r="G67" s="33"/>
       <c r="H67" s="31"/>
       <c r="I67" s="31" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="J67" s="33"/>
       <c r="K67" s="31"/>
       <c r="L67" s="37" t="s">
-        <v>788</v>
+        <v>794</v>
       </c>
       <c r="M67" s="29"/>
     </row>
@@ -5610,7 +5711,7 @@
       <c r="J94" s="33"/>
       <c r="K94" s="31"/>
       <c r="L94" s="37" t="s">
-        <v>704</v>
+        <v>762</v>
       </c>
       <c r="M94" s="29"/>
     </row>
@@ -5653,7 +5754,7 @@
       <c r="J96" s="33"/>
       <c r="K96" s="31"/>
       <c r="L96" s="37" t="s">
-        <v>704</v>
+        <v>762</v>
       </c>
       <c r="M96" s="29"/>
     </row>
@@ -10069,7 +10170,7 @@
       </c>
       <c r="G297" s="33"/>
       <c r="H297" s="31"/>
-      <c r="I297" s="36" t="s">
+      <c r="I297" s="31" t="s">
         <v>506</v>
       </c>
       <c r="J297" s="33"/>
@@ -10299,7 +10400,7 @@
       </c>
       <c r="M307" s="29"/>
     </row>
-    <row r="308" spans="2:13">
+    <row r="308" spans="2:13" ht="45">
       <c r="B308" s="16"/>
       <c r="C308" s="36" t="s">
         <v>528</v>
@@ -10312,12 +10413,12 @@
       <c r="G308" s="33"/>
       <c r="H308" s="31"/>
       <c r="I308" s="31" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="J308" s="33"/>
       <c r="K308" s="31"/>
       <c r="L308" s="37" t="s">
-        <v>759</v>
+        <v>793</v>
       </c>
       <c r="M308" s="29"/>
     </row>
@@ -12508,7 +12609,7 @@
       </c>
       <c r="F411">
         <f>Sheet1!E619</f>
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G411" s="29"/>
       <c r="L411" s="48" t="s">
@@ -12518,13 +12619,13 @@
     <row r="412" spans="2:13" ht="47.25" customHeight="1">
       <c r="B412" s="44"/>
       <c r="C412" s="58" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D412" s="56"/>
       <c r="E412" s="56"/>
       <c r="F412" s="45">
         <f>Sheet1!H619</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G412" s="46"/>
       <c r="L412" s="52" t="s">
@@ -12535,7 +12636,7 @@
     <row r="413" spans="2:13" ht="46.5" customHeight="1">
       <c r="B413" s="16"/>
       <c r="C413" s="57" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="D413" s="57"/>
       <c r="E413" s="57"/>
@@ -12669,7 +12770,7 @@
     <row r="427" spans="2:13" ht="15" customHeight="1">
       <c r="B427" s="16"/>
       <c r="C427" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="M427" s="29"/>
     </row>
@@ -12704,33 +12805,36 @@
     <mergeCell ref="F422:L424"/>
   </mergeCells>
   <conditionalFormatting sqref="L201:L203 G13:H398 I13:I402 C13:F402">
-    <cfRule type="containsText" dxfId="6" priority="19" operator="containsText" text="Not supported">
+    <cfRule type="containsText" dxfId="7" priority="21" operator="containsText" text="Not supported">
       <formula>NOT(ISERROR(SEARCH("Not supported",C13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C422:C442 B13:B442 C13:C419 C218:F218 C226:F226 C330:F330 D13:I442">
-    <cfRule type="containsText" dxfId="5" priority="18" operator="containsText" text="Can be converted">
+    <cfRule type="containsText" dxfId="6" priority="20" operator="containsText" text="Can be converted">
       <formula>NOT(ISERROR(SEARCH("Can be converted",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:M43 C62">
-    <cfRule type="expression" dxfId="4" priority="15">
+    <cfRule type="expression" dxfId="5" priority="17">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="16">
+    <cfRule type="expression" dxfId="4" priority="18">
       <formula>"MOD(ROW;2)=1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="17">
+    <cfRule type="expression" dxfId="3" priority="19">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:M402">
-    <cfRule type="expression" dxfId="1" priority="14">
-      <formula>MOD(ROW(),2)=1</formula>
+    <cfRule type="expression" dxfId="2" priority="15">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="16">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13:I402 C13:C402">
-    <cfRule type="expression" dxfId="0" priority="13">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>NOT(ISERR(SEARCH("1:1 conv",INDIRECT(ADDRESS(ROW(),12)))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12768,7 +12872,7 @@
         <v>781</v>
       </c>
       <c r="I5" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="J5" t="s">
         <v>780</v>
@@ -14849,7 +14953,7 @@
       <c r="D60" t="str">
         <f>functions_excel!L67</f>
         <v xml:space="preserve">Name of function changed.
-note: unit conversion function in Excel is named CONVERT, while in OOo it is named CONVERT_ADD ***. It is important not to confuse it with Ooo CONVERT, which converts European currencies. </v>
+note: unit conversion function in Excel is named CONVERT, while in OOo it is named CONVERT_ADD. It is important not to confuse it with Ooo CONVERT, which converts European currencies. </v>
       </c>
       <c r="E60">
         <f t="shared" si="1"/>
@@ -15879,11 +15983,11 @@
       </c>
       <c r="D87" t="str">
         <f>functions_excel!L94</f>
-        <v>1:1 conversion</v>
+        <v>Name changed only</v>
       </c>
       <c r="E87">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H87">
         <f t="shared" si="8"/>
@@ -15955,11 +16059,11 @@
       </c>
       <c r="D89" t="str">
         <f>functions_excel!L96</f>
-        <v>1:1 conversion</v>
+        <v>Name changed only</v>
       </c>
       <c r="E89">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H89">
         <f t="shared" si="8"/>
@@ -24007,7 +24111,7 @@
     <row r="301" spans="2:12">
       <c r="B301" t="str">
         <f>functions_excel!I308</f>
-        <v>Not supported</v>
+        <v>Can be converted</v>
       </c>
       <c r="C301">
         <f t="shared" si="24"/>
@@ -24015,7 +24119,8 @@
       </c>
       <c r="D301" t="str">
         <f>functions_excel!L308</f>
-        <v>Microsoft Office Excel only function</v>
+        <v>Can be converted to OpenOffice.org Calc according to following formula:
+RANDBETWEEN(A1,A2) = A1+INT(RAND(A2))</v>
       </c>
       <c r="E301">
         <f t="shared" si="25"/>
@@ -24023,11 +24128,11 @@
       </c>
       <c r="H301">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I301">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J301" t="str">
         <f>functions_excel!C308</f>
@@ -35924,15 +36029,15 @@
       </c>
       <c r="E619">
         <f>SUM(E6:E618)</f>
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H619">
         <f>SUM(H6:H618)</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I619">
         <f>SUM(I6:I618)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K619">
         <f>SUM(K6:K618)</f>

</xml_diff>